<commit_message>
adicionei arquivo de todo
</commit_message>
<xml_diff>
--- a/carteira-export.xlsx
+++ b/carteira-export.xlsx
@@ -1,18 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Carteira" sheetId="1" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="Carteira"/>
   </sheets>
   <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="37">
   <si>
     <t>Data operação</t>
   </si>
@@ -128,12 +130,15 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -154,307 +159,618 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" xfId="0" applyProtection="1"/>
+  <cellXfs count="3">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr lastClr="000000" val="windowText"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F818D"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin scaled="1" ang="16200000"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin scaled="1" ang="16200000"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="9500"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot rev="0" lon="0" lat="0"/>
+            </a:camera>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="0" t="s">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="0" t="s">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+      <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="G2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="J2" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" s="0" t="s">
+      <c r="H2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="0" t="s">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+      <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="F3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="G3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="K3" s="0" t="s">
+      <c r="H3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="0" t="s">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+      <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="F4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="0" t="s">
+      <c r="G4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="I4" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="J4" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="K4" s="0" t="s">
+      <c r="H4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="0" t="s">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+      <c r="A5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="0" t="s">
+      <c r="F5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G5" s="0" t="s">
+      <c r="G5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="I5" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="J5" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="K5" s="0" t="s">
+      <c r="H5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K5" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="0" t="s">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+      <c r="A6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="E6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="0" t="s">
+      <c r="F6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G6" s="0" t="s">
+      <c r="G6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H6" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="I6" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="J6" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="K6" s="0" t="s">
+      <c r="H6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K6" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="0" t="s">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+      <c r="A7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="E7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="0" t="s">
+      <c r="F7" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G7" s="0" t="s">
+      <c r="G7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H7" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="I7" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="J7" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="K7" s="0" t="s">
+      <c r="H7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K7" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="0" t="s">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+      <c r="A8" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="E8" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F8" s="0" t="s">
+      <c r="F8" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G8" s="0" t="s">
+      <c r="G8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="I8" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="J8" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="K8" s="0" t="s">
+      <c r="H8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K8" s="1" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
-  <headerFooter/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>